<commit_message>
put stuff into folders
</commit_message>
<xml_diff>
--- a/Equipment Summary.xlsx
+++ b/Equipment Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cbba6bb91481d9cf/Classes/CHEM E 485/Pontes_Ramos_Gao_Carpenter_485Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathanael\OneDrive\Classes\CHEM E 485\Pontes_Ramos_Gao_Carpenter_485Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="201" documentId="8_{B6292292-11EC-4752-8384-8F4105BC60A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F42B9832-D3C2-4669-B8C1-95C76AAAAA0B}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="8_{B6292292-11EC-4752-8384-8F4105BC60A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{75C327DA-95FF-41FA-BE62-67064B5F6026}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4628AA1-6D19-4550-85E3-7FDBB945C8C6}"/>
   </bookViews>
@@ -329,13 +329,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>18820</xdr:colOff>
+      <xdr:colOff>216940</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>563231</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>151751</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>149644</xdr:rowOff>
     </xdr:to>
@@ -360,7 +360,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9863860" y="0"/>
+          <a:off x="10061980" y="0"/>
           <a:ext cx="3592411" cy="4721644"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -718,7 +718,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J24" sqref="J24"/>
+      <selection pane="topRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
capcost equip and utilities
</commit_message>
<xml_diff>
--- a/Equipment Summary.xlsx
+++ b/Equipment Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathanael\OneDrive\Classes\CHEM E 485\Pontes_Ramos_Gao_Carpenter_485Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="8_{B6292292-11EC-4752-8384-8F4105BC60A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{75C327DA-95FF-41FA-BE62-67064B5F6026}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{B6292292-11EC-4752-8384-8F4105BC60A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF2BD241-C24E-4A97-B409-7D626BAC980F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4628AA1-6D19-4550-85E3-7FDBB945C8C6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
   <si>
     <t>TK-801</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>centrifugal (between T-801 and T-802, not used)</t>
+  </si>
+  <si>
+    <t>Heat Duty [kW]</t>
   </si>
 </sst>
 </file>
@@ -328,14 +331,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>216940</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>201700</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>151751</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>136511</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>149644</xdr:rowOff>
     </xdr:to>
@@ -360,7 +363,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10061980" y="0"/>
+          <a:off x="11265940" y="0"/>
           <a:ext cx="3592411" cy="4721644"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -372,13 +375,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>119074</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>500145</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>161243</xdr:rowOff>
@@ -714,11 +717,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EACAF4D-5FDA-4CEA-9023-83E3B5913271}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J15" sqref="J15"/>
+      <selection pane="topRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,9 +731,10 @@
     <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D1" s="7" t="s">
         <v>50</v>
       </c>
@@ -744,16 +748,17 @@
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="7"/>
+      <c r="O1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="7"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" s="7"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -788,25 +793,28 @@
         <v>67</v>
       </c>
       <c r="L2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" t="s">
         <v>54</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>55</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>48</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>49</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -820,7 +828,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -834,7 +842,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -851,7 +859,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -868,7 +876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -885,7 +893,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -902,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -919,7 +927,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -938,11 +946,15 @@
       <c r="K10" s="3">
         <v>3390000</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="2">
+        <f>K10/1000</f>
+        <v>3390</v>
+      </c>
+      <c r="M10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -958,11 +970,15 @@
       <c r="K11" s="3">
         <v>5310000</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="2">
+        <f t="shared" ref="L11:L16" si="0">K11/1000</f>
+        <v>5310</v>
+      </c>
+      <c r="M11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -981,11 +997,15 @@
       <c r="K12" s="3">
         <v>-1930000</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="2">
+        <f t="shared" si="0"/>
+        <v>-1930</v>
+      </c>
+      <c r="M12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1004,11 +1024,15 @@
       <c r="K13" s="3">
         <v>2360000</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="2">
+        <f t="shared" si="0"/>
+        <v>2360</v>
+      </c>
+      <c r="M13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1027,11 +1051,15 @@
       <c r="K14" s="3">
         <v>-1610000</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2">
+        <f t="shared" si="0"/>
+        <v>-1610</v>
+      </c>
+      <c r="M14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1050,11 +1078,15 @@
       <c r="K15" s="3">
         <v>1610000</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="2">
+        <f t="shared" si="0"/>
+        <v>1610</v>
+      </c>
+      <c r="M15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1070,14 +1102,18 @@
       <c r="K16" s="3">
         <v>2670000</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="2">
+        <f t="shared" si="0"/>
+        <v>2670</v>
+      </c>
+      <c r="M16" t="s">
         <v>64</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1096,14 +1132,14 @@
       <c r="H17">
         <v>65</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>63</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1126,14 +1162,14 @@
       <c r="I18" s="1">
         <v>0.5</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>59</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1156,14 +1192,14 @@
       <c r="I19" s="1">
         <v>0.5</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>61</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1180,7 +1216,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1199,8 +1235,9 @@
       <c r="K21" s="3">
         <v>71100</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1217,7 +1254,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1236,10 +1273,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
     <mergeCell ref="D1:G1"/>
-    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="I1:N1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Putting Equipment Summary in PFD Readme
</commit_message>
<xml_diff>
--- a/Equipment Summary.xlsx
+++ b/Equipment Summary.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathanael\OneDrive\Classes\CHEM E 485\Pontes_Ramos_Gao_Carpenter_485Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\College 19-20\Folder 485 - Process Design\Pontes_Ramos_Gao_Carpenter_485Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="8_{B6292292-11EC-4752-8384-8F4105BC60A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF2BD241-C24E-4A97-B409-7D626BAC980F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2D19FA-D3D9-4ED0-9B24-18C83F0B9A5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4628AA1-6D19-4550-85E3-7FDBB945C8C6}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{D4628AA1-6D19-4550-85E3-7FDBB945C8C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="138">
   <si>
     <t>TK-801</t>
   </si>
@@ -255,6 +254,198 @@
   </si>
   <si>
     <t>Heat Duty [kW]</t>
+  </si>
+  <si>
+    <t>Heat Exchangers</t>
+  </si>
+  <si>
+    <t>E-801:</t>
+  </si>
+  <si>
+    <t>E-802:</t>
+  </si>
+  <si>
+    <t>E-803:</t>
+  </si>
+  <si>
+    <t>E-804:</t>
+  </si>
+  <si>
+    <t>E-805:</t>
+  </si>
+  <si>
+    <t>E-806:</t>
+  </si>
+  <si>
+    <t>Pumps</t>
+  </si>
+  <si>
+    <t>P-801:</t>
+  </si>
+  <si>
+    <t>Centrifugal pump/electric drive</t>
+  </si>
+  <si>
+    <t>Carbon Steel</t>
+  </si>
+  <si>
+    <t>P-802:</t>
+  </si>
+  <si>
+    <t>Tanks (not shown on PFD)</t>
+  </si>
+  <si>
+    <t>TK-801:</t>
+  </si>
+  <si>
+    <t>storage tank for benzene.</t>
+  </si>
+  <si>
+    <t>TK-802:</t>
+  </si>
+  <si>
+    <t>storage tank for propylene.</t>
+  </si>
+  <si>
+    <t>Fired Heater</t>
+  </si>
+  <si>
+    <t>Reactor</t>
+  </si>
+  <si>
+    <t>R-801:</t>
+  </si>
+  <si>
+    <t>375 tubes, 7.62 cm ID, 6 m long</t>
+  </si>
+  <si>
+    <t>Distillation Columns</t>
+  </si>
+  <si>
+    <t>T-801:</t>
+  </si>
+  <si>
+    <t>Carbon steel</t>
+  </si>
+  <si>
+    <t>14 carbon steel trays with total condenser and reboiler</t>
+  </si>
+  <si>
+    <t>T-802:</t>
+  </si>
+  <si>
+    <t>18 carbon steel trays with total condenser and reboiler</t>
+  </si>
+  <si>
+    <t>Vessels</t>
+  </si>
+  <si>
+    <t>V-801:</t>
+  </si>
+  <si>
+    <t>Horizontal</t>
+  </si>
+  <si>
+    <t>V-802:</t>
+  </si>
+  <si>
+    <t>Vertical</t>
+  </si>
+  <si>
+    <t>V-803:</t>
+  </si>
+  <si>
+    <t>V-804:</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Area [m^2]</t>
+  </si>
+  <si>
+    <t>Overall Heat Transfer Coeff [W/(m^2 C)]</t>
+  </si>
+  <si>
+    <t>13.5 in desubcooling zone, 7.3 in vaporizing zone</t>
+  </si>
+  <si>
+    <t>Heat Transferred [W]</t>
+  </si>
+  <si>
+    <t>600 in desubcooling zone, 1500 in vaporizing zone</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>1-2 Floating head heat exchanger, hps, 2 zones</t>
+  </si>
+  <si>
+    <t>1-2 Floating head heat exchanger, cw</t>
+  </si>
+  <si>
+    <t>1-2 Floating head heat exchanger, mps</t>
+  </si>
+  <si>
+    <t>1-2 Floating head heat exchanger, hps</t>
+  </si>
+  <si>
+    <t>Actual Power [kW]</t>
+  </si>
+  <si>
+    <t>Volume [m^3]</t>
+  </si>
+  <si>
+    <t>Heat Load [MJ/h]</t>
+  </si>
+  <si>
+    <t>Design Heat Load [MJ/h]</t>
+  </si>
+  <si>
+    <t>Thermal Efficiency</t>
+  </si>
+  <si>
+    <t>Max Pressure [bar]</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>Pressure [bar]</t>
+  </si>
+  <si>
+    <t>Temperature [C]</t>
+  </si>
+  <si>
+    <t>shell-and-tube packed bed, catalyst parameters are specified by Appendix C.6.</t>
+  </si>
+  <si>
+    <t>Tray Efficiency</t>
+  </si>
+  <si>
+    <t>Feed Tray</t>
+  </si>
+  <si>
+    <t>Reflux Ratio</t>
+  </si>
+  <si>
+    <t>Tray Spacing [in]</t>
+  </si>
+  <si>
+    <t>Height [m]</t>
+  </si>
+  <si>
+    <t>Diameter [m]</t>
+  </si>
+  <si>
+    <t>Orientation</t>
+  </si>
+  <si>
+    <t>L/D</t>
+  </si>
+  <si>
+    <t>Volume [m]</t>
   </si>
 </sst>
 </file>
@@ -264,7 +455,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +469,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -287,7 +523,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -295,11 +531,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -309,6 +560,35 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,22 +999,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EACAF4D-5FDA-4CEA-9023-83E3B5913271}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L19" sqref="L19"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.3515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.3515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.87890625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.64453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.5">
       <c r="D1" s="7" t="s">
         <v>50</v>
       </c>
@@ -758,7 +1038,7 @@
       </c>
       <c r="R1" s="7"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -814,7 +1094,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -828,7 +1108,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -842,7 +1122,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -859,7 +1139,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -876,7 +1156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -893,7 +1173,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -910,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -927,7 +1207,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -954,7 +1234,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -978,7 +1258,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1005,7 +1285,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1032,7 +1312,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1059,7 +1339,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1086,7 +1366,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1113,7 +1393,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1139,7 +1419,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1169,7 +1449,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1199,7 +1479,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1216,7 +1496,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1237,7 +1517,7 @@
       </c>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1254,7 +1534,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1282,4 +1562,554 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABCD9DC-CA73-431E-BB38-2733F333996E}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="15.9375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9" style="9" customWidth="1"/>
+    <col min="3" max="3" width="24.76171875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="25.29296875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="18.5859375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.64453125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="19.64453125" style="9" customWidth="1"/>
+    <col min="8" max="9" width="15.46875" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="8.5859375" customWidth="1"/>
+    <col min="12" max="12" width="12.703125" customWidth="1"/>
+    <col min="13" max="13" width="13.76171875" customWidth="1"/>
+    <col min="14" max="14" width="17.64453125" customWidth="1"/>
+    <col min="15" max="15" width="12.05859375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="44.35" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" s="17">
+        <v>3390000</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="16">
+        <v>3</v>
+      </c>
+      <c r="O2" s="16">
+        <v>6.46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="16">
+        <v>533</v>
+      </c>
+      <c r="F3" s="16">
+        <v>850</v>
+      </c>
+      <c r="G3" s="17">
+        <v>5310000</v>
+      </c>
+      <c r="J3" s="15"/>
+      <c r="K3" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="16">
+        <v>5.2</v>
+      </c>
+      <c r="O3" s="16">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="16">
+        <v>151</v>
+      </c>
+      <c r="F4" s="16">
+        <v>450</v>
+      </c>
+      <c r="G4" s="17">
+        <v>-1930000</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="N4" s="16">
+        <v>2.5</v>
+      </c>
+      <c r="O4" s="16">
+        <v>8.0399999999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="16">
+        <v>405</v>
+      </c>
+      <c r="F5" s="16">
+        <v>750</v>
+      </c>
+      <c r="G5" s="17">
+        <v>2360000</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" s="16">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="O5" s="16">
+        <v>13.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="16">
+        <v>24</v>
+      </c>
+      <c r="F6" s="16">
+        <v>450</v>
+      </c>
+      <c r="G6" s="17">
+        <v>-1610000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="16">
+        <v>64</v>
+      </c>
+      <c r="F7" s="16">
+        <v>750</v>
+      </c>
+      <c r="G7" s="17">
+        <v>1610000</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="J8" s="15"/>
+      <c r="K8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="M8" s="16">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="M9" s="16">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="16">
+        <v>9641</v>
+      </c>
+      <c r="D10" s="18">
+        <v>10000</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="G10" s="16">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J11" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="N12" s="16">
+        <v>24.24</v>
+      </c>
+      <c r="O12" s="19">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="16">
+        <v>6.5</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="16">
+        <v>30.75</v>
+      </c>
+      <c r="G13" s="16">
+        <v>365</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="N13" s="16">
+        <v>7</v>
+      </c>
+      <c r="O13" s="19">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="16">
+        <v>7</v>
+      </c>
+      <c r="G16" s="16">
+        <v>0.44</v>
+      </c>
+      <c r="H16" s="16">
+        <v>24</v>
+      </c>
+      <c r="I16" s="16">
+        <v>8.69</v>
+      </c>
+      <c r="J16" s="16">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="K16" s="16">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="16">
+        <v>9</v>
+      </c>
+      <c r="G17" s="16">
+        <v>0.63</v>
+      </c>
+      <c r="H17" s="16">
+        <v>24</v>
+      </c>
+      <c r="I17" s="16">
+        <v>11.13</v>
+      </c>
+      <c r="J17" s="16">
+        <v>1.26</v>
+      </c>
+      <c r="K17" s="16">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M19" s="11"/>
+    </row>
+    <row r="20" spans="1:13" ht="36.35" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="21" spans="1:13" ht="34.35" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>